<commit_message>
Calcualte HQM score order top 50 and aamout shares to buy
</commit_message>
<xml_diff>
--- a/Recommended_equalstrat_trades.xlsx
+++ b/Recommended_equalstrat_trades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>Ticker</t>
   </si>
@@ -218,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="$0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,14 +229,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -283,14 +275,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,9 +589,13 @@
     <col min="7" max="7" width="18.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,601 +606,604 @@
         <v>64</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2">
-        <v>133.53</v>
+        <v>133.36</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <v>-0.1371724510490707</v>
+        <v>-0.1387272868317343</v>
       </c>
       <c r="E2" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F2" s="3">
-        <v>-0.0005135133209332357</v>
+        <v>-0.0005239438313275781</v>
       </c>
       <c r="G2" s="3">
         <v>79.67806841046277</v>
       </c>
       <c r="H2" s="3">
-        <v>0.09564254716254063</v>
+        <v>0.0962495565784135</v>
       </c>
       <c r="I2" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J2">
-        <v>0.02516419546176569</v>
-      </c>
-      <c r="K2">
+      <c r="J2" s="3">
+        <v>0.02430878589347394</v>
+      </c>
+      <c r="K2" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>69.3158953722334</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>12.59</v>
+        <v>12.24</v>
       </c>
       <c r="C3" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3">
-        <v>-0.3884006653667201</v>
+        <v>-0.3883706538660946</v>
       </c>
       <c r="E3" s="3">
         <v>69.01408450704226</v>
       </c>
       <c r="F3" s="3">
-        <v>-0.273651717640352</v>
+        <v>-0.275017062233869</v>
       </c>
       <c r="G3" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H3" s="3">
-        <v>-0.08714581880603865</v>
+        <v>-0.08693653097757195</v>
       </c>
       <c r="I3" s="3">
         <v>53.52112676056338</v>
       </c>
-      <c r="J3">
-        <v>-0.03876051952054766</v>
-      </c>
-      <c r="K3">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L3">
+      <c r="J3" s="3">
+        <v>-0.03789130670954981</v>
+      </c>
+      <c r="K3" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L3" s="3">
         <v>68.30985915492958</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2">
-        <v>166.69</v>
+        <v>167.74</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>-0.1964937901643517</v>
+        <v>-0.1998064871623493</v>
       </c>
       <c r="E4" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F4" s="3">
-        <v>-0.2205664579678709</v>
+        <v>-0.2192364739433665</v>
       </c>
       <c r="G4" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H4" s="3">
-        <v>-0.0844126257589901</v>
+        <v>-0.08341148780207112</v>
       </c>
       <c r="I4" s="3">
         <v>53.52112676056338</v>
       </c>
-      <c r="J4">
-        <v>-0.04062718220104329</v>
-      </c>
-      <c r="K4">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L4">
+      <c r="J4" s="3">
+        <v>-0.04039680944137961</v>
+      </c>
+      <c r="K4" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L4" s="3">
         <v>68.36016096579476</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>142.75</v>
+        <v>140.69</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>0.03031512785127565</v>
+        <v>0.03062463930224323</v>
       </c>
       <c r="E5" s="3">
         <v>71.0261569416499</v>
       </c>
       <c r="F5" s="3">
-        <v>-0.158560864196725</v>
+        <v>-0.157105475576322</v>
       </c>
       <c r="G5" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H5" s="3">
-        <v>0.01955905719387437</v>
+        <v>0.01900096011271723</v>
       </c>
       <c r="I5" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J5">
-        <v>-0.05940563810030141</v>
-      </c>
-      <c r="K5">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L5">
+      <c r="J5" s="3">
+        <v>-0.06013956575403536</v>
+      </c>
+      <c r="K5" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L5" s="3">
         <v>69.26559356136821</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>141.51</v>
+        <v>140.33</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>0.3515509664947363</v>
+        <v>0.3490722861189968</v>
       </c>
       <c r="E6" s="3">
         <v>71.62977867203219</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.1591231525020339</v>
+        <v>-0.1609761752046069</v>
       </c>
       <c r="G6" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H6" s="3">
-        <v>-0.07314528802490071</v>
+        <v>-0.07203188085769638</v>
       </c>
       <c r="I6" s="3">
         <v>53.72233400402415</v>
       </c>
-      <c r="J6">
-        <v>0.02019602498782382</v>
-      </c>
-      <c r="K6">
+      <c r="J6" s="3">
+        <v>0.01988605552494332</v>
+      </c>
+      <c r="K6" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <v>69.41649899396378</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>139.06</v>
+        <v>137.36</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>0.2183265286255471</v>
+        <v>0.2197626007334871</v>
       </c>
       <c r="E7" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F7" s="3">
-        <v>-0.1140332883351679</v>
+        <v>-0.1099011431848619</v>
       </c>
       <c r="G7" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H7" s="3">
-        <v>0.003636248070533865</v>
+        <v>0.003643918657489865</v>
       </c>
       <c r="I7" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J7">
-        <v>-0.04187826709797109</v>
-      </c>
-      <c r="K7">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L7">
+      <c r="J7" s="3">
+        <v>-0.0423255185875291</v>
+      </c>
+      <c r="K7" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L7" s="3">
         <v>69.3158953722334</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>258.53</v>
+        <v>257.67</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>-0.2130697058991307</v>
+        <v>-0.2119710345840866</v>
       </c>
       <c r="E8" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.1538741397820238</v>
+        <v>-0.1540225189581052</v>
       </c>
       <c r="G8" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H8" s="3">
-        <v>0.05620754483517074</v>
+        <v>0.0548076218481858</v>
       </c>
       <c r="I8" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J8">
-        <v>0.01280707592479965</v>
-      </c>
-      <c r="K8">
+      <c r="J8" s="3">
+        <v>0.0126760284312519</v>
+      </c>
+      <c r="K8" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L8">
-        <v>69.21529175050301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="L8" s="3">
+        <v>69.21529175050301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="2">
-        <v>104.66</v>
+        <v>105.47</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>-0.1066385271351855</v>
+        <v>-0.10704502525723</v>
       </c>
       <c r="E9" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.1432059061943842</v>
+        <v>-0.1405516372568906</v>
       </c>
       <c r="G9" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H9" s="3">
-        <v>-0.0555350112652034</v>
+        <v>-0.05357894084561048</v>
       </c>
       <c r="I9" s="3">
         <v>53.72233400402415</v>
       </c>
-      <c r="J9">
-        <v>-0.002613691321711285</v>
-      </c>
-      <c r="K9">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L9">
+      <c r="J9" s="3">
+        <v>-0.00264046615269141</v>
+      </c>
+      <c r="K9" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L9" s="3">
         <v>68.41046277665995</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="2">
-        <v>260.8</v>
+        <v>265.93</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
       </c>
       <c r="D10" s="3">
-        <v>-0.1688605942078216</v>
+        <v>-0.1658473928430537</v>
       </c>
       <c r="E10" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.2121344133738788</v>
+        <v>-0.2083107314571274</v>
       </c>
       <c r="G10" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H10" s="3">
-        <v>-0.0200733220096766</v>
+        <v>-0.02041016489011736</v>
       </c>
       <c r="I10" s="3">
         <v>53.72233400402415</v>
       </c>
-      <c r="J10">
-        <v>-0.04955608891675602</v>
-      </c>
-      <c r="K10">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L10">
+      <c r="J10" s="3">
+        <v>-0.05143116693221914</v>
+      </c>
+      <c r="K10" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L10" s="3">
         <v>68.41046277665995</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>300.9</v>
+        <v>302.3</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>-0.4978667812039345</v>
+        <v>-0.4994602310311278</v>
       </c>
       <c r="E11" s="3">
         <v>69.01408450704226</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.341262839844764</v>
+        <v>-0.3420905281745718</v>
       </c>
       <c r="G11" s="3">
         <v>78.67203219315896</v>
       </c>
       <c r="H11" s="3">
-        <v>-0.2305084619792449</v>
+        <v>-0.2209079583185699</v>
       </c>
       <c r="I11" s="3">
         <v>53.11871227364185</v>
       </c>
-      <c r="J11">
-        <v>-0.1936429508304243</v>
-      </c>
-      <c r="K11">
+      <c r="J11" s="3">
+        <v>-0.195932083322331</v>
+      </c>
+      <c r="K11" s="3">
         <v>70.62374245472837</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="3">
         <v>67.85714285714286</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="2">
-        <v>145.2</v>
+        <v>149.74</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>-0.07499736643432871</v>
+        <v>-0.07432981567006988</v>
       </c>
       <c r="E12" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F12" s="3">
-        <v>-0.05071553481452791</v>
+        <v>-0.05106964707125811</v>
       </c>
       <c r="G12" s="3">
         <v>79.67806841046277</v>
       </c>
       <c r="H12" s="3">
-        <v>0.05076719553340815</v>
+        <v>0.04984821729832078</v>
       </c>
       <c r="I12" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J12">
-        <v>0.01849976488962722</v>
-      </c>
-      <c r="K12">
+      <c r="J12" s="3">
+        <v>0.01901170696025996</v>
+      </c>
+      <c r="K12" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="3">
         <v>69.3158953722334</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>88.48999999999999</v>
+        <v>85.56999999999999</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
       </c>
       <c r="D13" s="3">
-        <v>0.407742840585204</v>
+        <v>0.4128576404787969</v>
       </c>
       <c r="E13" s="3">
         <v>71.83098591549296</v>
       </c>
       <c r="F13" s="3">
-        <v>-0.06921828758204349</v>
+        <v>-0.06807498512071848</v>
       </c>
       <c r="G13" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H13" s="3">
-        <v>0.1959761759847157</v>
+        <v>0.1933262810814278</v>
       </c>
       <c r="I13" s="3">
-        <v>56.33802816901409</v>
-      </c>
-      <c r="J13">
-        <v>0.0006002596187988732</v>
-      </c>
-      <c r="K13">
+        <v>56.13682092555332</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.0006123455427676642</v>
+      </c>
+      <c r="K13" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L13">
-        <v>70.12072434607646</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="L13" s="3">
+        <v>70.07042253521126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="2">
-        <v>234.19</v>
+        <v>236.38</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
       </c>
       <c r="D14" s="3">
-        <v>0.169687152911784</v>
+        <v>0.172345642401207</v>
       </c>
       <c r="E14" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F14" s="3">
-        <v>-0.003280844777094782</v>
+        <v>-0.003220273897063127</v>
       </c>
       <c r="G14" s="3">
         <v>79.67806841046277</v>
       </c>
       <c r="H14" s="3">
-        <v>0.08716375438245838</v>
+        <v>0.08907284831601041</v>
       </c>
       <c r="I14" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J14">
-        <v>-0.00979040262250659</v>
-      </c>
-      <c r="K14">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L14">
+      <c r="J14" s="3">
+        <v>-0.00945897203047791</v>
+      </c>
+      <c r="K14" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L14" s="3">
         <v>69.41649899396378</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="2">
-        <v>203.78</v>
+        <v>198.43</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
       </c>
       <c r="D15" s="3">
-        <v>-0.2607965943784542</v>
+        <v>-0.2616660241381045</v>
       </c>
       <c r="E15" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F15" s="3">
-        <v>0.00981919395733568</v>
+        <v>0.009601386148090521</v>
       </c>
       <c r="G15" s="3">
         <v>81.28772635814889</v>
       </c>
       <c r="H15" s="3">
-        <v>0.169116832539185</v>
+        <v>0.1684176628879273</v>
       </c>
       <c r="I15" s="3">
         <v>56.13682092555332</v>
       </c>
-      <c r="J15">
-        <v>0.04007480044715376</v>
-      </c>
-      <c r="K15">
+      <c r="J15" s="3">
+        <v>0.04023825402746564</v>
+      </c>
+      <c r="K15" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="3">
         <v>69.91951710261569</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="2">
-        <v>78.66</v>
+        <v>80.48999999999999</v>
       </c>
       <c r="C16" s="2">
         <v>2</v>
       </c>
       <c r="D16" s="3">
-        <v>-0.03183436173534576</v>
+        <v>-0.03174734821005515</v>
       </c>
       <c r="E16" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F16" s="3">
-        <v>-0.1887219987066034</v>
+        <v>-0.1873698578469261</v>
       </c>
       <c r="G16" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H16" s="3">
-        <v>-0.112516088943237</v>
+        <v>-0.114225905688167</v>
       </c>
       <c r="I16" s="3">
-        <v>53.52112676056338</v>
-      </c>
-      <c r="J16">
-        <v>-0.1467245861570725</v>
-      </c>
-      <c r="K16">
+        <v>53.31991951710262</v>
+      </c>
+      <c r="J16" s="3">
+        <v>-0.1503965287842312</v>
+      </c>
+      <c r="K16" s="3">
         <v>71.0261569416499</v>
       </c>
-      <c r="L16">
-        <v>68.25955734406439</v>
+      <c r="L16" s="3">
+        <v>68.2092555331992</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1221,30 +1217,30 @@
         <v>2</v>
       </c>
       <c r="D17" s="3">
-        <v>0.0352983474377691</v>
+        <v>0.03529947705882891</v>
       </c>
       <c r="E17" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F17" s="3">
-        <v>-0.1858236004389777</v>
+        <v>-0.1870021202974699</v>
       </c>
       <c r="G17" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H17" s="3">
-        <v>-0.1057843850572781</v>
+        <v>-0.1064952052339937</v>
       </c>
       <c r="I17" s="3">
         <v>53.52112676056338</v>
       </c>
-      <c r="J17">
-        <v>-0.1719990371355566</v>
-      </c>
-      <c r="K17">
+      <c r="J17" s="3">
+        <v>-0.169533937913555</v>
+      </c>
+      <c r="K17" s="3">
         <v>70.82494969818913</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="3">
         <v>68.7122736418511</v>
       </c>
     </row>
@@ -1253,36 +1249,36 @@
         <v>28</v>
       </c>
       <c r="B18" s="2">
-        <v>25.98</v>
+        <v>25.36</v>
       </c>
       <c r="C18" s="2">
         <v>7</v>
       </c>
       <c r="D18" s="3">
-        <v>0.119477098761936</v>
+        <v>0.1194770432610449</v>
       </c>
       <c r="E18" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F18" s="3">
-        <v>0.01202427143784369</v>
+        <v>0.01172365139465936</v>
       </c>
       <c r="G18" s="3">
         <v>81.28772635814889</v>
       </c>
       <c r="H18" s="3">
-        <v>0.2218420726179605</v>
+        <v>0.2237023287758255</v>
       </c>
       <c r="I18" s="3">
         <v>56.33802816901409</v>
       </c>
-      <c r="J18">
-        <v>-0.0259206605247031</v>
-      </c>
-      <c r="K18">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L18">
+      <c r="J18" s="3">
+        <v>-0.0258880458331958</v>
+      </c>
+      <c r="K18" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L18" s="3">
         <v>70.07042253521126</v>
       </c>
     </row>
@@ -1291,36 +1287,36 @@
         <v>29</v>
       </c>
       <c r="B19" s="2">
-        <v>58.51</v>
+        <v>57.91</v>
       </c>
       <c r="C19" s="2">
         <v>3</v>
       </c>
       <c r="D19" s="3">
-        <v>0.1426470325026775</v>
+        <v>0.1437764008045699</v>
       </c>
       <c r="E19" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F19" s="3">
-        <v>-0.0792636394626894</v>
+        <v>-0.0802234626706381</v>
       </c>
       <c r="G19" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H19" s="3">
-        <v>0.06460940726365459</v>
+        <v>0.06594629117147603</v>
       </c>
       <c r="I19" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J19">
-        <v>-0.006677429959256343</v>
-      </c>
-      <c r="K19">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L19">
+      <c r="J19" s="3">
+        <v>-0.006582474802650905</v>
+      </c>
+      <c r="K19" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L19" s="3">
         <v>69.3158953722334</v>
       </c>
     </row>
@@ -1329,36 +1325,36 @@
         <v>30</v>
       </c>
       <c r="B20" s="2">
-        <v>50.47</v>
+        <v>51.4</v>
       </c>
       <c r="C20" s="2">
         <v>3</v>
       </c>
       <c r="D20" s="3">
-        <v>-0.09429452412456162</v>
+        <v>-0.09625281807759309</v>
       </c>
       <c r="E20" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F20" s="3">
-        <v>-0.1729474901782814</v>
+        <v>-0.1764005868255932</v>
       </c>
       <c r="G20" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H20" s="3">
-        <v>0.001618343127819076</v>
+        <v>0.001617044992462642</v>
       </c>
       <c r="I20" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J20">
-        <v>-0.0259283053139912</v>
-      </c>
-      <c r="K20">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L20">
+      <c r="J20" s="3">
+        <v>-0.02529679774209836</v>
+      </c>
+      <c r="K20" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L20" s="3">
         <v>68.81287726358148</v>
       </c>
     </row>
@@ -1367,36 +1363,36 @@
         <v>31</v>
       </c>
       <c r="B21" s="2">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="C21" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3">
-        <v>0.03280933454324724</v>
+        <v>0.03291554298609565</v>
       </c>
       <c r="E21" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F21" s="3">
-        <v>0.03852773300614714</v>
+        <v>0.03758213892375085</v>
       </c>
       <c r="G21" s="3">
         <v>81.28772635814889</v>
       </c>
       <c r="H21" s="3">
-        <v>0.09129672739985693</v>
+        <v>0.09273408824746217</v>
       </c>
       <c r="I21" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J21">
-        <v>-0.1815377306776974</v>
-      </c>
-      <c r="K21">
+      <c r="J21" s="3">
+        <v>-0.1857948289013074</v>
+      </c>
+      <c r="K21" s="3">
         <v>70.82494969818913</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="3">
         <v>69.66800804828974</v>
       </c>
     </row>
@@ -1405,36 +1401,36 @@
         <v>32</v>
       </c>
       <c r="B22" s="2">
-        <v>147.78</v>
+        <v>147.79</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>-0.05968295601848016</v>
+        <v>-0.05820965329621323</v>
       </c>
       <c r="E22" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F22" s="3">
-        <v>-0.188679899688414</v>
+        <v>-0.182828713924581</v>
       </c>
       <c r="G22" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H22" s="3">
-        <v>-0.1383031877192218</v>
+        <v>-0.1417945750461587</v>
       </c>
       <c r="I22" s="3">
         <v>53.11871227364185</v>
       </c>
-      <c r="J22">
-        <v>-0.05672773181288254</v>
-      </c>
-      <c r="K22">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L22">
+      <c r="J22" s="3">
+        <v>-0.05730079252819579</v>
+      </c>
+      <c r="K22" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L22" s="3">
         <v>68.25955734406439</v>
       </c>
     </row>
@@ -1443,36 +1439,36 @@
         <v>33</v>
       </c>
       <c r="B23" s="2">
-        <v>176.89</v>
+        <v>176.51</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
       </c>
       <c r="D23" s="3">
-        <v>0.1953103181396036</v>
+        <v>0.191543049336049</v>
       </c>
       <c r="E23" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F23" s="3">
-        <v>0.00646634458251956</v>
+        <v>0.006548085045299655</v>
       </c>
       <c r="G23" s="3">
         <v>81.28772635814889</v>
       </c>
       <c r="H23" s="3">
-        <v>0.06950132188168899</v>
+        <v>0.07021535894365966</v>
       </c>
       <c r="I23" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J23">
-        <v>-0.01043311883525286</v>
-      </c>
-      <c r="K23">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L23">
+      <c r="J23" s="3">
+        <v>-0.01038469965354021</v>
+      </c>
+      <c r="K23" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L23" s="3">
         <v>69.81891348088531</v>
       </c>
     </row>
@@ -1481,36 +1477,36 @@
         <v>34</v>
       </c>
       <c r="B24" s="2">
-        <v>82.81</v>
+        <v>85.41</v>
       </c>
       <c r="C24" s="2">
         <v>2</v>
       </c>
       <c r="D24" s="3">
-        <v>-0.1917681811389224</v>
+        <v>-0.1929377245241191</v>
       </c>
       <c r="E24" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F24" s="3">
-        <v>-0.3071574404369178</v>
+        <v>-0.3059858077493866</v>
       </c>
       <c r="G24" s="3">
         <v>79.07444668008048</v>
       </c>
       <c r="H24" s="3">
-        <v>-0.08796981110813815</v>
+        <v>-0.08891115469928326</v>
       </c>
       <c r="I24" s="3">
         <v>53.52112676056338</v>
       </c>
-      <c r="J24">
-        <v>-0.0496891740284055</v>
-      </c>
-      <c r="K24">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L24">
+      <c r="J24" s="3">
+        <v>-0.04850490865438723</v>
+      </c>
+      <c r="K24" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L24" s="3">
         <v>68.30985915492958</v>
       </c>
     </row>
@@ -1519,36 +1515,36 @@
         <v>35</v>
       </c>
       <c r="B25" s="2">
-        <v>282.09</v>
+        <v>284.03</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
       </c>
       <c r="D25" s="3">
-        <v>0.2780978251451341</v>
+        <v>0.2745734317436855</v>
       </c>
       <c r="E25" s="3">
         <v>71.42857142857143</v>
       </c>
       <c r="F25" s="3">
-        <v>0.3332732631496094</v>
+        <v>0.3402469869122191</v>
       </c>
       <c r="G25" s="3">
         <v>81.48893360160966</v>
       </c>
       <c r="H25" s="3">
-        <v>0.421086985202747</v>
+        <v>0.4361926827217203</v>
       </c>
       <c r="I25" s="3">
         <v>57.34406438631791</v>
       </c>
-      <c r="J25">
-        <v>0.05609737093113302</v>
-      </c>
-      <c r="K25">
+      <c r="J25" s="3">
+        <v>0.05490356616800802</v>
+      </c>
+      <c r="K25" s="3">
         <v>73.2394366197183</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="3">
         <v>70.87525150905432</v>
       </c>
     </row>
@@ -1557,37 +1553,37 @@
         <v>36</v>
       </c>
       <c r="B26" s="2">
-        <v>219.25</v>
+        <v>212.59</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>-0.6774982589846247</v>
+        <v>-0.6745292648948152</v>
       </c>
       <c r="E26" s="3">
         <v>68.81287726358148</v>
       </c>
       <c r="F26" s="3">
-        <v>-0.472924326395225</v>
+        <v>-0.47919069829744</v>
       </c>
       <c r="G26" s="3">
         <v>78.26961770623743</v>
       </c>
       <c r="H26" s="3">
-        <v>-0.1124182746777087</v>
+        <v>-0.1139389451478971</v>
       </c>
       <c r="I26" s="3">
-        <v>53.52112676056338</v>
-      </c>
-      <c r="J26">
-        <v>-0.07143676176989108</v>
-      </c>
-      <c r="K26">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L26">
-        <v>68.00804828973843</v>
+        <v>53.31991951710262</v>
+      </c>
+      <c r="J26" s="3">
+        <v>-0.06960878505877756</v>
+      </c>
+      <c r="K26" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L26" s="3">
+        <v>67.95774647887325</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1595,36 +1591,36 @@
         <v>37</v>
       </c>
       <c r="B27" s="2">
-        <v>42.34</v>
+        <v>42.56</v>
       </c>
       <c r="C27" s="2">
         <v>4</v>
       </c>
       <c r="D27" s="3">
-        <v>-0.3092029782052795</v>
+        <v>-0.3111279137262106</v>
       </c>
       <c r="E27" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F27" s="3">
-        <v>-0.2396016684197974</v>
+        <v>-0.2304754595544327</v>
       </c>
       <c r="G27" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H27" s="3">
-        <v>0.03390673494293509</v>
+        <v>0.03487526427166773</v>
       </c>
       <c r="I27" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J27">
-        <v>-0.03391117738802176</v>
-      </c>
-      <c r="K27">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L27">
+      <c r="J27" s="3">
+        <v>-0.03420490644468236</v>
+      </c>
+      <c r="K27" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L27" s="3">
         <v>68.81287726358148</v>
       </c>
     </row>
@@ -1633,36 +1629,36 @@
         <v>38</v>
       </c>
       <c r="B28" s="2">
-        <v>136.48</v>
+        <v>132.04</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="D28" s="3">
-        <v>0.05348311894877963</v>
+        <v>0.05392184565202895</v>
       </c>
       <c r="E28" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F28" s="3">
-        <v>-0.04936314553048798</v>
+        <v>-0.04953180732181198</v>
       </c>
       <c r="G28" s="3">
         <v>79.67806841046277</v>
       </c>
       <c r="H28" s="3">
-        <v>0.00236365326957879</v>
+        <v>0.002377365252707497</v>
       </c>
       <c r="I28" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J28">
-        <v>0.07479337422611571</v>
-      </c>
-      <c r="K28">
+      <c r="J28" s="3">
+        <v>0.0751427231827375</v>
+      </c>
+      <c r="K28" s="3">
         <v>73.44064386317908</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="3">
         <v>69.91951710261569</v>
       </c>
     </row>
@@ -1671,36 +1667,36 @@
         <v>39</v>
       </c>
       <c r="B29" s="2">
-        <v>93.55</v>
+        <v>94.14</v>
       </c>
       <c r="C29" s="2">
         <v>2</v>
       </c>
       <c r="D29" s="3">
-        <v>-0.261804492325112</v>
+        <v>-0.2591799301798658</v>
       </c>
       <c r="E29" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F29" s="3">
-        <v>-0.1137508343236896</v>
+        <v>-0.1112933224298839</v>
       </c>
       <c r="G29" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H29" s="3">
-        <v>-0.0610361794484392</v>
+        <v>-0.0589315235017081</v>
       </c>
       <c r="I29" s="3">
         <v>53.72233400402415</v>
       </c>
-      <c r="J29">
-        <v>0.001939855663139182</v>
-      </c>
-      <c r="K29">
+      <c r="J29" s="3">
+        <v>0.001968713038591933</v>
+      </c>
+      <c r="K29" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="3">
         <v>68.81287726358148</v>
       </c>
     </row>
@@ -1709,7 +1705,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="2">
-        <v>188.2</v>
+        <v>183.7</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -1732,13 +1728,13 @@
       <c r="I30" s="3">
         <v>54.62776659959759</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="3">
         <v>0</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="3">
         <v>72.33400402414487</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="3">
         <v>69.41649899396378</v>
       </c>
     </row>
@@ -1747,36 +1743,36 @@
         <v>41</v>
       </c>
       <c r="B31" s="2">
-        <v>85.23999999999999</v>
+        <v>82.98999999999999</v>
       </c>
       <c r="C31" s="2">
         <v>2</v>
       </c>
       <c r="D31" s="3">
-        <v>-0.306354460306843</v>
+        <v>-0.300522945062866</v>
       </c>
       <c r="E31" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F31" s="3">
-        <v>-0.2611873905566935</v>
+        <v>-0.2694383088095705</v>
       </c>
       <c r="G31" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H31" s="3">
-        <v>0.02153329923035504</v>
+        <v>0.02070149764756929</v>
       </c>
       <c r="I31" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J31">
-        <v>-0.02426831014091171</v>
-      </c>
-      <c r="K31">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L31">
+      <c r="J31" s="3">
+        <v>-0.02413689854627145</v>
+      </c>
+      <c r="K31" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L31" s="3">
         <v>68.81287726358148</v>
       </c>
     </row>
@@ -1785,37 +1781,37 @@
         <v>42</v>
       </c>
       <c r="B32" s="2">
-        <v>11.28</v>
+        <v>10.81</v>
       </c>
       <c r="C32" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="3">
-        <v>-0.03071575313796353</v>
+        <v>-0.02986225449615584</v>
       </c>
       <c r="E32" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F32" s="3">
-        <v>-0.01901273512520381</v>
+        <v>-0.01878309049102303</v>
       </c>
       <c r="G32" s="3">
         <v>79.67806841046277</v>
       </c>
       <c r="H32" s="3">
-        <v>-0.1215712004105574</v>
+        <v>-0.1202771426042714</v>
       </c>
       <c r="I32" s="3">
-        <v>53.11871227364185</v>
-      </c>
-      <c r="J32">
-        <v>-0.05874827956330181</v>
-      </c>
-      <c r="K32">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L32">
-        <v>68.36016096579476</v>
+        <v>53.31991951710262</v>
+      </c>
+      <c r="J32" s="3">
+        <v>-0.05648247155483284</v>
+      </c>
+      <c r="K32" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L32" s="3">
+        <v>68.41046277665995</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1823,36 +1819,36 @@
         <v>43</v>
       </c>
       <c r="B33" s="2">
-        <v>61.3</v>
+        <v>59.3</v>
       </c>
       <c r="C33" s="2">
         <v>3</v>
       </c>
       <c r="D33" s="3">
-        <v>-0.3530785983424656</v>
+        <v>-0.3512531633790177</v>
       </c>
       <c r="E33" s="3">
         <v>69.01408450704226</v>
       </c>
       <c r="F33" s="3">
-        <v>-0.3568647605853044</v>
+        <v>-0.3493033148135581</v>
       </c>
       <c r="G33" s="3">
         <v>78.67203219315896</v>
       </c>
       <c r="H33" s="3">
-        <v>-0.1033046869384179</v>
+        <v>-0.1039902053632394</v>
       </c>
       <c r="I33" s="3">
         <v>53.52112676056338</v>
       </c>
-      <c r="J33">
-        <v>-0.1399968234056835</v>
-      </c>
-      <c r="K33">
+      <c r="J33" s="3">
+        <v>-0.1386770756662467</v>
+      </c>
+      <c r="K33" s="3">
         <v>71.0261569416499</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="3">
         <v>68.05835010060362</v>
       </c>
     </row>
@@ -1861,36 +1857,36 @@
         <v>44</v>
       </c>
       <c r="B34" s="2">
-        <v>117.26</v>
+        <v>118.89</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
       </c>
       <c r="D34" s="3">
-        <v>-0.04025341453770827</v>
+        <v>-0.04049220102922842</v>
       </c>
       <c r="E34" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F34" s="3">
-        <v>-0.09209676935599856</v>
+        <v>-0.09291194376791878</v>
       </c>
       <c r="G34" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H34" s="3">
-        <v>0.06925486235229186</v>
+        <v>0.06752621191608668</v>
       </c>
       <c r="I34" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J34">
-        <v>0.003539609597531246</v>
-      </c>
-      <c r="K34">
+      <c r="J34" s="3">
+        <v>0.003443444587773687</v>
+      </c>
+      <c r="K34" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="3">
         <v>69.21529175050301</v>
       </c>
     </row>
@@ -1899,36 +1895,36 @@
         <v>45</v>
       </c>
       <c r="B35" s="2">
-        <v>238.86</v>
+        <v>231.76</v>
       </c>
       <c r="C35" s="2">
         <v>0</v>
       </c>
       <c r="D35" s="3">
-        <v>0.1422610584685202</v>
+        <v>0.140399357207379</v>
       </c>
       <c r="E35" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F35" s="3">
-        <v>-0.06343162195620947</v>
+        <v>-0.06434029780174791</v>
       </c>
       <c r="G35" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H35" s="3">
-        <v>-0.05162903454689621</v>
+        <v>-0.05136602065974087</v>
       </c>
       <c r="I35" s="3">
         <v>53.72233400402415</v>
       </c>
-      <c r="J35">
-        <v>-0.04803798529877042</v>
-      </c>
-      <c r="K35">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L35">
+      <c r="J35" s="3">
+        <v>-0.04675881029527759</v>
+      </c>
+      <c r="K35" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L35" s="3">
         <v>68.91348088531187</v>
       </c>
     </row>
@@ -1937,36 +1933,36 @@
         <v>46</v>
       </c>
       <c r="B36" s="2">
-        <v>281.02</v>
+        <v>280.46</v>
       </c>
       <c r="C36" s="2">
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>0.02439743317220089</v>
+        <v>0.02363697225548655</v>
       </c>
       <c r="E36" s="3">
         <v>71.0261569416499</v>
       </c>
       <c r="F36" s="3">
-        <v>-0.05038761488593969</v>
+        <v>-0.05210767179202618</v>
       </c>
       <c r="G36" s="3">
         <v>79.67806841046277</v>
       </c>
       <c r="H36" s="3">
-        <v>0.1879326323912569</v>
+        <v>0.1844585831962308</v>
       </c>
       <c r="I36" s="3">
         <v>56.13682092555332</v>
       </c>
-      <c r="J36">
-        <v>0.02444464042499564</v>
-      </c>
-      <c r="K36">
+      <c r="J36" s="3">
+        <v>0.02474690840518435</v>
+      </c>
+      <c r="K36" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="3">
         <v>69.96981891348088</v>
       </c>
     </row>
@@ -1975,36 +1971,36 @@
         <v>47</v>
       </c>
       <c r="B37" s="2">
-        <v>201.51</v>
+        <v>202.29</v>
       </c>
       <c r="C37" s="2">
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <v>-0.2369721799611247</v>
+        <v>-0.2393391837528639</v>
       </c>
       <c r="E37" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F37" s="3">
-        <v>-0.2425792977350495</v>
+        <v>-0.2421583818172608</v>
       </c>
       <c r="G37" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H37" s="3">
-        <v>-0.222566363699134</v>
+        <v>-0.2169461717873225</v>
       </c>
       <c r="I37" s="3">
         <v>53.11871227364185</v>
       </c>
-      <c r="J37">
-        <v>-0.2070581740271033</v>
-      </c>
-      <c r="K37">
+      <c r="J37" s="3">
+        <v>-0.2052277525823424</v>
+      </c>
+      <c r="K37" s="3">
         <v>70.62374245472837</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="3">
         <v>68.05835010060362</v>
       </c>
     </row>
@@ -2013,36 +2009,36 @@
         <v>48</v>
       </c>
       <c r="B38" s="2">
-        <v>119.68</v>
+        <v>116.49</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
       </c>
       <c r="D38" s="3">
-        <v>-0.2634913582096223</v>
+        <v>-0.2717075248098549</v>
       </c>
       <c r="E38" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F38" s="3">
-        <v>-0.2480848130298811</v>
+        <v>-0.245016567039989</v>
       </c>
       <c r="G38" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H38" s="3">
-        <v>0.0533647461021531</v>
+        <v>0.05268107219683441</v>
       </c>
       <c r="I38" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J38">
-        <v>-0.0465384355578121</v>
-      </c>
-      <c r="K38">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L38">
+      <c r="J38" s="3">
+        <v>-0.0465364232381162</v>
+      </c>
+      <c r="K38" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L38" s="3">
         <v>68.81287726358148</v>
       </c>
     </row>
@@ -2051,37 +2047,37 @@
         <v>49</v>
       </c>
       <c r="B39" s="2">
-        <v>119.69</v>
+        <v>116.8</v>
       </c>
       <c r="C39" s="2">
         <v>1</v>
       </c>
       <c r="D39" s="3">
-        <v>0.3933953932860641</v>
+        <v>0.3902571712303651</v>
       </c>
       <c r="E39" s="3">
         <v>71.62977867203219</v>
       </c>
       <c r="F39" s="3">
-        <v>-0.07990822357797539</v>
+        <v>-0.07737756099761743</v>
       </c>
       <c r="G39" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H39" s="3">
-        <v>0.2448341005586714</v>
+        <v>0.2430784447588887</v>
       </c>
       <c r="I39" s="3">
-        <v>56.74044265593562</v>
-      </c>
-      <c r="J39">
-        <v>0.03760068632930399</v>
-      </c>
-      <c r="K39">
+        <v>56.53923541247485</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0.037405831640506</v>
+      </c>
+      <c r="K39" s="3">
         <v>73.03822937625755</v>
       </c>
-      <c r="L39">
-        <v>70.17102615694165</v>
+      <c r="L39" s="3">
+        <v>70.12072434607646</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2089,36 +2085,36 @@
         <v>50</v>
       </c>
       <c r="B40" s="2">
-        <v>219.89</v>
+        <v>223.47</v>
       </c>
       <c r="C40" s="2">
         <v>0</v>
       </c>
       <c r="D40" s="3">
-        <v>-0.3396182334886211</v>
+        <v>-0.3326935291228703</v>
       </c>
       <c r="E40" s="3">
         <v>69.01408450704226</v>
       </c>
       <c r="F40" s="3">
-        <v>-0.2605299221619755</v>
+        <v>-0.2572808459269561</v>
       </c>
       <c r="G40" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H40" s="3">
-        <v>-0.06429972820092512</v>
+        <v>-0.06346259658127715</v>
       </c>
       <c r="I40" s="3">
         <v>53.72233400402415</v>
       </c>
-      <c r="J40">
-        <v>-0.0390580825132669</v>
-      </c>
-      <c r="K40">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L40">
+      <c r="J40" s="3">
+        <v>-0.0377362169790008</v>
+      </c>
+      <c r="K40" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L40" s="3">
         <v>68.36016096579476</v>
       </c>
     </row>
@@ -2127,36 +2123,36 @@
         <v>51</v>
       </c>
       <c r="B41" s="2">
-        <v>482.95</v>
+        <v>505.49</v>
       </c>
       <c r="C41" s="2">
         <v>0</v>
       </c>
       <c r="D41" s="3">
-        <v>0.2923890529157713</v>
+        <v>0.2911638837839043</v>
       </c>
       <c r="E41" s="3">
         <v>71.42857142857143</v>
       </c>
       <c r="F41" s="3">
-        <v>0.05667334943903383</v>
+        <v>0.05794641913114352</v>
       </c>
       <c r="G41" s="3">
         <v>81.28772635814889</v>
       </c>
       <c r="H41" s="3">
-        <v>0.00658380954202073</v>
+        <v>0.006398084545735001</v>
       </c>
       <c r="I41" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J41">
-        <v>-0.0708543299592878</v>
-      </c>
-      <c r="K41">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L41">
+      <c r="J41" s="3">
+        <v>-0.07403987248355438</v>
+      </c>
+      <c r="K41" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L41" s="3">
         <v>69.86921529175051</v>
       </c>
     </row>
@@ -2165,36 +2161,36 @@
         <v>52</v>
       </c>
       <c r="B42" s="2">
-        <v>281.37</v>
+        <v>281.22</v>
       </c>
       <c r="C42" s="2">
         <v>0</v>
       </c>
       <c r="D42" s="3">
-        <v>-0.02882157827980903</v>
+        <v>-0.02903885365377128</v>
       </c>
       <c r="E42" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F42" s="3">
-        <v>-0.150999935510324</v>
+        <v>-0.1509109847631048</v>
       </c>
       <c r="G42" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H42" s="3">
-        <v>0.006157820067258136</v>
+        <v>0.00610468936822145</v>
       </c>
       <c r="I42" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J42">
-        <v>-0.001830597777102508</v>
-      </c>
-      <c r="K42">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L42">
+      <c r="J42" s="3">
+        <v>-0.001898628334075061</v>
+      </c>
+      <c r="K42" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L42" s="3">
         <v>68.81287726358148</v>
       </c>
     </row>
@@ -2203,36 +2199,36 @@
         <v>53</v>
       </c>
       <c r="B43" s="2">
-        <v>51.4</v>
+        <v>50.3</v>
       </c>
       <c r="C43" s="2">
         <v>3</v>
       </c>
       <c r="D43" s="3">
-        <v>-0.1927477082008398</v>
+        <v>-0.1959997027742888</v>
       </c>
       <c r="E43" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F43" s="3">
-        <v>-0.2120202660441655</v>
+        <v>-0.2167318152345846</v>
       </c>
       <c r="G43" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H43" s="3">
-        <v>-0.121213986164739</v>
+        <v>-0.1234529302720158</v>
       </c>
       <c r="I43" s="3">
         <v>53.11871227364185</v>
       </c>
-      <c r="J43">
-        <v>-0.09510211233549749</v>
-      </c>
-      <c r="K43">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L43">
+      <c r="J43" s="3">
+        <v>-0.0943247546379528</v>
+      </c>
+      <c r="K43" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L43" s="3">
         <v>68.25955734406439</v>
       </c>
     </row>
@@ -2241,36 +2237,36 @@
         <v>54</v>
       </c>
       <c r="B44" s="2">
-        <v>43.448</v>
+        <v>42.74</v>
       </c>
       <c r="C44" s="2">
         <v>4</v>
       </c>
       <c r="D44" s="3">
-        <v>0.9488689163510534</v>
+        <v>0.9655809319298448</v>
       </c>
       <c r="E44" s="3">
         <v>72.63581488933602</v>
       </c>
       <c r="F44" s="3">
-        <v>0.04171974421031183</v>
+        <v>0.04079221761691424</v>
       </c>
       <c r="G44" s="3">
         <v>81.28772635814889</v>
       </c>
       <c r="H44" s="3">
-        <v>0.3251045994481589</v>
+        <v>0.3245921890282288</v>
       </c>
       <c r="I44" s="3">
         <v>56.94164989939638</v>
       </c>
-      <c r="J44">
-        <v>0.117651724204865</v>
-      </c>
-      <c r="K44">
+      <c r="J44" s="3">
+        <v>0.11684803842429</v>
+      </c>
+      <c r="K44" s="3">
         <v>73.64185110663983</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="3">
         <v>71.12676056338029</v>
       </c>
     </row>
@@ -2279,36 +2275,36 @@
         <v>55</v>
       </c>
       <c r="B45" s="2">
-        <v>242.41</v>
+        <v>233.25</v>
       </c>
       <c r="C45" s="2">
         <v>0</v>
       </c>
       <c r="D45" s="3">
-        <v>-0.06395173753703347</v>
+        <v>-0.06412084550955806</v>
       </c>
       <c r="E45" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F45" s="3">
-        <v>-0.03312881279411437</v>
+        <v>-0.03325484958758449</v>
       </c>
       <c r="G45" s="3">
         <v>79.67806841046277</v>
       </c>
       <c r="H45" s="3">
-        <v>0.01289331746364838</v>
+        <v>0.01317939398895965</v>
       </c>
       <c r="I45" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J45">
-        <v>-0.02431875879733905</v>
-      </c>
-      <c r="K45">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L45">
+      <c r="J45" s="3">
+        <v>-0.02451140684252494</v>
+      </c>
+      <c r="K45" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L45" s="3">
         <v>68.91348088531187</v>
       </c>
     </row>
@@ -2317,36 +2313,36 @@
         <v>56</v>
       </c>
       <c r="B46" s="2">
-        <v>72.54000000000001</v>
+        <v>72.20999999999999</v>
       </c>
       <c r="C46" s="2">
         <v>2</v>
       </c>
       <c r="D46" s="3">
-        <v>-0.01859113689008299</v>
+        <v>-0.01872283569878313</v>
       </c>
       <c r="E46" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F46" s="3">
-        <v>-0.003262567607448615</v>
+        <v>-0.003226860718044326</v>
       </c>
       <c r="G46" s="3">
         <v>79.67806841046277</v>
       </c>
       <c r="H46" s="3">
-        <v>0.1324271235343069</v>
+        <v>0.1298801535579248</v>
       </c>
       <c r="I46" s="3">
         <v>55.73440643863179</v>
       </c>
-      <c r="J46">
-        <v>-0.003129512374736282</v>
-      </c>
-      <c r="K46">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L46">
+      <c r="J46" s="3">
+        <v>-0.003107314895313589</v>
+      </c>
+      <c r="K46" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L46" s="3">
         <v>69.01408450704226</v>
       </c>
     </row>
@@ -2355,36 +2351,36 @@
         <v>57</v>
       </c>
       <c r="B47" s="2">
-        <v>87.01000000000001</v>
+        <v>86.98999999999999</v>
       </c>
       <c r="C47" s="2">
         <v>2</v>
       </c>
       <c r="D47" s="3">
-        <v>-0.442169396943885</v>
+        <v>-0.4540747932357644</v>
       </c>
       <c r="E47" s="3">
         <v>69.01408450704226</v>
       </c>
       <c r="F47" s="3">
-        <v>-0.2083773598484107</v>
+        <v>-0.2109825475429092</v>
       </c>
       <c r="G47" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H47" s="3">
-        <v>0.00954659231969248</v>
+        <v>0.009847038829633219</v>
       </c>
       <c r="I47" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J47">
-        <v>-0.006323947054908539</v>
-      </c>
-      <c r="K47">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L47">
+      <c r="J47" s="3">
+        <v>-0.006129120960600551</v>
+      </c>
+      <c r="K47" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L47" s="3">
         <v>68.76257545271631</v>
       </c>
     </row>
@@ -2393,36 +2389,36 @@
         <v>58</v>
       </c>
       <c r="B48" s="2">
-        <v>139.39</v>
+        <v>141.03</v>
       </c>
       <c r="C48" s="2">
         <v>1</v>
       </c>
       <c r="D48" s="3">
-        <v>-0.2764702850922697</v>
+        <v>-0.2790987384138769</v>
       </c>
       <c r="E48" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F48" s="3">
-        <v>-0.3140368644984015</v>
+        <v>-0.3195534402253698</v>
       </c>
       <c r="G48" s="3">
         <v>79.07444668008048</v>
       </c>
       <c r="H48" s="3">
-        <v>-0.06424081831284222</v>
+        <v>-0.063493172933721</v>
       </c>
       <c r="I48" s="3">
         <v>53.72233400402415</v>
       </c>
-      <c r="J48">
-        <v>-0.079764551323877</v>
-      </c>
-      <c r="K48">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L48">
+      <c r="J48" s="3">
+        <v>-0.0803120370350143</v>
+      </c>
+      <c r="K48" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L48" s="3">
         <v>68.36016096579476</v>
       </c>
     </row>
@@ -2431,36 +2427,36 @@
         <v>59</v>
       </c>
       <c r="B49" s="2">
-        <v>100.4</v>
+        <v>99.55</v>
       </c>
       <c r="C49" s="2">
         <v>1</v>
       </c>
       <c r="D49" s="3">
-        <v>0.1390740297998204</v>
+        <v>0.1456355343594019</v>
       </c>
       <c r="E49" s="3">
         <v>71.22736418511066</v>
       </c>
       <c r="F49" s="3">
-        <v>-0.1686058128521627</v>
+        <v>-0.1663579153668848</v>
       </c>
       <c r="G49" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H49" s="3">
-        <v>-0.1038060772843769</v>
+        <v>-0.1068072358998909</v>
       </c>
       <c r="I49" s="3">
         <v>53.52112676056338</v>
       </c>
-      <c r="J49">
-        <v>-0.1192701438946801</v>
-      </c>
-      <c r="K49">
+      <c r="J49" s="3">
+        <v>-0.1213445544148968</v>
+      </c>
+      <c r="K49" s="3">
         <v>71.0261569416499</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="3">
         <v>68.76257545271629</v>
       </c>
     </row>
@@ -2469,36 +2465,36 @@
         <v>60</v>
       </c>
       <c r="B50" s="2">
-        <v>76.09</v>
+        <v>73.98999999999999</v>
       </c>
       <c r="C50" s="2">
         <v>2</v>
       </c>
       <c r="D50" s="3">
-        <v>-0.04039273631924481</v>
+        <v>-0.0391435306797098</v>
       </c>
       <c r="E50" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F50" s="3">
-        <v>-0.07538956309539242</v>
+        <v>-0.07570604593388829</v>
       </c>
       <c r="G50" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H50" s="3">
-        <v>-0.05832778112721627</v>
+        <v>-0.05973528290035741</v>
       </c>
       <c r="I50" s="3">
         <v>53.72233400402415</v>
       </c>
-      <c r="J50">
-        <v>-0.04098313488352767</v>
-      </c>
-      <c r="K50">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L50">
+      <c r="J50" s="3">
+        <v>-0.04107554260488192</v>
+      </c>
+      <c r="K50" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L50" s="3">
         <v>68.41046277665995</v>
       </c>
     </row>
@@ -2507,36 +2503,36 @@
         <v>61</v>
       </c>
       <c r="B51" s="2">
-        <v>173.76</v>
+        <v>176.34</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
       </c>
       <c r="D51" s="3">
-        <v>-0.1952174543755422</v>
+        <v>-0.1967334475819018</v>
       </c>
       <c r="E51" s="3">
         <v>69.21529175050301</v>
       </c>
       <c r="F51" s="3">
-        <v>-0.293570956731398</v>
+        <v>-0.3009044939538361</v>
       </c>
       <c r="G51" s="3">
         <v>79.07444668008048</v>
       </c>
       <c r="H51" s="3">
-        <v>-0.0788028892859442</v>
+        <v>-0.07682892473365352</v>
       </c>
       <c r="I51" s="3">
         <v>53.52112676056338</v>
       </c>
-      <c r="J51">
-        <v>-0.135943827455059</v>
-      </c>
-      <c r="K51">
+      <c r="J51" s="3">
+        <v>-0.1356219489241313</v>
+      </c>
+      <c r="K51" s="3">
         <v>71.0261569416499</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="3">
         <v>68.2092555331992</v>
       </c>
     </row>
@@ -2545,36 +2541,36 @@
         <v>62</v>
       </c>
       <c r="B52" s="2">
-        <v>479.44</v>
+        <v>460.7</v>
       </c>
       <c r="C52" s="2">
         <v>0</v>
       </c>
       <c r="D52" s="3">
-        <v>0.002349289446444405</v>
+        <v>0.002305664661246801</v>
       </c>
       <c r="E52" s="3">
         <v>70.82494969818913</v>
       </c>
       <c r="F52" s="3">
-        <v>-0.1997170564742805</v>
+        <v>-0.2041923129056044</v>
       </c>
       <c r="G52" s="3">
         <v>79.27565392354124</v>
       </c>
       <c r="H52" s="3">
-        <v>0.001952997413314039</v>
+        <v>0.001978060377714246</v>
       </c>
       <c r="I52" s="3">
         <v>55.33199195171026</v>
       </c>
-      <c r="J52">
-        <v>-0.03055357907402008</v>
-      </c>
-      <c r="K52">
-        <v>71.42857142857143</v>
-      </c>
-      <c r="L52">
+      <c r="J52" s="3">
+        <v>-0.03093754938329815</v>
+      </c>
+      <c r="K52" s="3">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="L52" s="3">
         <v>69.21529175050301</v>
       </c>
     </row>

</xml_diff>